<commit_message>
Fix 'add knowledge from chat' and add 'update knowledge base'
</commit_message>
<xml_diff>
--- a/knowledge_base.xlsx
+++ b/knowledge_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\990180\ChatbotAI-LLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46AE240-1AC8-460C-B22C-5D1B10133341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720D2C80-6D9C-4DFB-AFE9-7F0D273E444C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="310" windowWidth="9800" windowHeight="9770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6590" yWindow="310" windowWidth="12610" windowHeight="9770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="246">
   <si>
     <t>product_name</t>
   </si>
@@ -745,13 +745,19 @@
     <t>http://benziro.com/home/delivery/jasa-instalasi-listrik-murah-benziro</t>
   </si>
   <si>
+    <t>Ruijie RG-ES216GC 16-Port Gigabit Cloud Managed Switch</t>
+  </si>
+  <si>
     <t>Tokopedia</t>
   </si>
   <si>
     <t>https://www.tokopedia.com/sinshekomputer/ruijie-rg-es216gc-16-port-gigabit-ethernet-cloud-managed-switch)</t>
   </si>
   <si>
-    <t>Ruijie RG-ES216GC 16-Port Gigabit Cloud Managed Switch</t>
+    <t>Mini UPS 5V 2A 3000mAh Automatic Charging for Router WiFi CCTV</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/megatronsby/mini-ups-5v-2a-3000mah-automatic-charging-for-router-wifi-cctv)</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2916,16 +2922,30 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B129">
         <v>1400000</v>
       </c>
       <c r="C129" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D129" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130">
+        <v>189900</v>
+      </c>
+      <c r="C130" t="s">
         <v>242</v>
+      </c>
+      <c r="D130" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>